<commit_message>
finished no duplicate fellapp and fixed user generator
</commit_message>
<xml_diff>
--- a/Scanorders2/src/Oleg/UserdirectoryBundle/Util/UsersFullTest.xlsx
+++ b/Scanorders2/src/Oleg/UserdirectoryBundle/Util/UsersFullTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="51195" windowHeight="24240"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="51195" windowHeight="24180"/>
   </bookViews>
   <sheets>
     <sheet name="owssvr.dll" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="103">
   <si>
     <t>A</t>
   </si>
@@ -66,36 +66,12 @@
     <t>Dr.</t>
   </si>
   <si>
-    <t>Hematopathology Faculty</t>
-  </si>
-  <si>
-    <t>Cesarman</t>
-  </si>
-  <si>
-    <t>Ethel</t>
-  </si>
-  <si>
-    <t>ecesarm@med.cornell.edu</t>
-  </si>
-  <si>
-    <t>(212) 746-8838</t>
-  </si>
-  <si>
-    <t>(212) 746-4483</t>
-  </si>
-  <si>
-    <t>C-410B</t>
-  </si>
-  <si>
     <t>Assistants</t>
   </si>
   <si>
     <t>Degree</t>
   </si>
   <si>
-    <t>MD; PhD</t>
-  </si>
-  <si>
     <t>Intercom</t>
   </si>
   <si>
@@ -108,9 +84,6 @@
     <t>CWID</t>
   </si>
   <si>
-    <t>Professor of Pathology and Laboratory Medicine</t>
-  </si>
-  <si>
     <t>NYPH Code</t>
   </si>
   <si>
@@ -132,30 +105,9 @@
     <t>License expiration</t>
   </si>
   <si>
-    <t>Attending Pathologist</t>
-  </si>
-  <si>
-    <t>NY</t>
-  </si>
-  <si>
-    <t>CE018</t>
-  </si>
-  <si>
-    <t>187177-1</t>
-  </si>
-  <si>
-    <t>3/1/1994</t>
-  </si>
-  <si>
-    <t>9/30/2015</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Viral Oncogenesis</t>
-  </si>
-  <si>
     <t>Research Lab Title</t>
   </si>
   <si>
@@ -171,12 +123,6 @@
     <t>Board Certification - Recertification Date</t>
   </si>
   <si>
-    <t>Anatomic Pathology; Molecular Genetic Pathology</t>
-  </si>
-  <si>
-    <t>11/20/1991; 9/24/2007</t>
-  </si>
-  <si>
     <t>Administrative Comment - Category</t>
   </si>
   <si>
@@ -186,15 +132,6 @@
     <t>Administrative Comment - Comment</t>
   </si>
   <si>
-    <t>Faculty Database - Donna</t>
-  </si>
-  <si>
-    <t>Special Appointment Notes</t>
-  </si>
-  <si>
-    <t>2007 Professor</t>
-  </si>
-  <si>
     <t>Identifier - Type</t>
   </si>
   <si>
@@ -219,15 +156,6 @@
     <t>Certificate of Qualification - Expiration Date</t>
   </si>
   <si>
-    <t>CESAE1</t>
-  </si>
-  <si>
-    <t>CQP90583</t>
-  </si>
-  <si>
-    <t>2/8/2016</t>
-  </si>
-  <si>
     <t>CLIA - Number</t>
   </si>
   <si>
@@ -237,18 +165,6 @@
     <t>PFI</t>
   </si>
   <si>
-    <t>NPI;EIN</t>
-  </si>
-  <si>
-    <t>1770523987; 200-08-083</t>
-  </si>
-  <si>
-    <t>null; 12/31/2017</t>
-  </si>
-  <si>
-    <t>Assistant Director, Molecular Hematopathology</t>
-  </si>
-  <si>
     <t>Administrative - Institution</t>
   </si>
   <si>
@@ -309,27 +225,9 @@
     <t>Academic Appointment - Faculty Track</t>
   </si>
   <si>
-    <t xml:space="preserve">New York-Presbyterian Hospital; New York-Presbyterian Hospital; </t>
-  </si>
-  <si>
-    <t>Yes; Yes</t>
-  </si>
-  <si>
     <t>Clinical; Research</t>
   </si>
   <si>
-    <t>Pathology and Laboratory Medicine; Pathology and Laboratory Medicine</t>
-  </si>
-  <si>
-    <t>Hematopathology; Molecular and Genomic Pathology</t>
-  </si>
-  <si>
-    <t>Molecular Hematopathology; Molecular Hematopathology</t>
-  </si>
-  <si>
-    <t>Weill Cornell Medical College; Weill Cornell Medical College; Weill Cornell Medical College</t>
-  </si>
-  <si>
     <t>POPS Link</t>
   </si>
   <si>
@@ -339,19 +237,109 @@
     <t>Pubmed Link</t>
   </si>
   <si>
-    <t>http://vivo.med.cornell.edu/display/cwid-ecesarm</t>
-  </si>
-  <si>
-    <t>http://www.ncbi.nlm.nih.gov/pubmed?term=Cesarman%20E%5BAuthor%5D&amp;cauthor=true&amp;cauthor_uid=22507788</t>
-  </si>
-  <si>
     <t>Certifying Board Organization</t>
   </si>
   <si>
-    <t>American Board of Pathology;American Board of Pathology</t>
-  </si>
-  <si>
-    <t>ecesarm4</t>
+    <t>Anatomic Pathology Faculty</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>Medical Director of Informatics</t>
+  </si>
+  <si>
+    <t>New York-Presbyterian Hospital</t>
+  </si>
+  <si>
+    <t>Pathology and Laboratory Medicine</t>
+  </si>
+  <si>
+    <t>Pathology Informatics</t>
+  </si>
+  <si>
+    <t>Assistant Professor of Pathology and Laboratory Medicine; Assistant Professor of Public Health</t>
+  </si>
+  <si>
+    <t>3/1/2010</t>
+  </si>
+  <si>
+    <t>(646) 962-2997; (646) 592-3803; (212) 746-5820</t>
+  </si>
+  <si>
+    <t>(212) 746-2113</t>
+  </si>
+  <si>
+    <t>K-505</t>
+  </si>
+  <si>
+    <t>vib9020@med.cornell.edu</t>
+  </si>
+  <si>
+    <t>EIN</t>
+  </si>
+  <si>
+    <t>200-31-063</t>
+  </si>
+  <si>
+    <t>http://weillcornell.org/vbrodsky</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/pubmed?term=Brodsky%20V%5BAuthor%5D&amp;cauthor=true&amp;cauthor_uid=23024889</t>
+  </si>
+  <si>
+    <t>http://vivo.med.cornell.edu/display/cwid-vib9020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. </t>
+  </si>
+  <si>
+    <t>Alain</t>
+  </si>
+  <si>
+    <t>Vice Chairman, Anatomic Pathology</t>
+  </si>
+  <si>
+    <t>Weill Cornell Medical College</t>
+  </si>
+  <si>
+    <t>Anatomic Pathology</t>
+  </si>
+  <si>
+    <t>Assistant Professor of Pathology and Laboratory Medicine (Interim)</t>
+  </si>
+  <si>
+    <t>Assistant Professor of Pathology and Laboratory Medicine (interim)</t>
+  </si>
+  <si>
+    <t>(212) 746-5769</t>
+  </si>
+  <si>
+    <t>16573</t>
+  </si>
+  <si>
+    <t>Starr-1000</t>
+  </si>
+  <si>
+    <t>alb9003@med.cornell.edu</t>
+  </si>
+  <si>
+    <t>Gaud, Melody</t>
+  </si>
+  <si>
+    <t>vib9020Test3</t>
+  </si>
+  <si>
+    <t>Brodsky3</t>
+  </si>
+  <si>
+    <t>alb9003Test4</t>
+  </si>
+  <si>
+    <t>Borczuk4</t>
   </si>
 </sst>
 </file>
@@ -511,12 +499,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -530,6 +512,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -719,12 +707,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDEBF7"/>
-        <bgColor rgb="FFDDEBF7"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -839,6 +827,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="288">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1130,7 +1129,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1147,25 +1146,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1174,11 +1170,35 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1472,23 +1492,16 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="58">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+  <dxfs count="66">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1536,7 +1549,40 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1557,7 +1603,142 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1582,115 +1763,8 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
+          <bgColor indexed="65"/>
+        </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1712,7 +1786,130 @@
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1734,86 +1931,6 @@
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
@@ -1897,6 +2014,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1922,6 +2049,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -1957,16 +2087,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1992,6 +2112,165 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2009,50 +2288,19 @@
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2075,6 +2323,36 @@
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="5" tint="0.79998168889431442"/>
@@ -2084,67 +2362,11 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
@@ -2163,34 +2385,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr.dll" displayName="Table_owssvr.dll" ref="A1:BM2" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr.dll" displayName="Table_owssvr.dll" ref="A1:BM2" totalsRowShown="0" headerRowDxfId="65">
   <autoFilter ref="A1:BM2"/>
   <sortState ref="A2:BL356">
     <sortCondition ref="D1:D356"/>
   </sortState>
   <tableColumns count="65">
-    <tableColumn id="1" name="A" dataDxfId="55"/>
-    <tableColumn id="2" name="Primary Group" dataDxfId="54"/>
-    <tableColumn id="5" name="Salut." dataDxfId="53"/>
-    <tableColumn id="6" name="Last Name" dataDxfId="52"/>
-    <tableColumn id="7" name="First Name" dataDxfId="51"/>
-    <tableColumn id="45" name="Middle Name" dataDxfId="50"/>
-    <tableColumn id="22" name="Degree" dataDxfId="49"/>
-    <tableColumn id="54" name="Employee Type" dataDxfId="48"/>
-    <tableColumn id="28" name="Administrative Title" dataDxfId="47"/>
-    <tableColumn id="44" name="Administrative - Institution" dataDxfId="46"/>
-    <tableColumn id="31" name="Administrative - Department" dataDxfId="45"/>
-    <tableColumn id="24" name="Administrative - Division" dataDxfId="44"/>
-    <tableColumn id="25" name="Administrative - Service" dataDxfId="43"/>
-    <tableColumn id="33" name="Administrative - Head of this Department"/>
-    <tableColumn id="35" name="Administrative - Head of this Division"/>
-    <tableColumn id="34" name="Administrative - Head of this Service"/>
-    <tableColumn id="20" name="Medical Staff Appointment (MSA) Title"/>
-    <tableColumn id="62" name="MSA - Institution"/>
-    <tableColumn id="61" name="MSA - Department"/>
-    <tableColumn id="43" name="MSA - Division"/>
-    <tableColumn id="42" name="MSA - Service"/>
-    <tableColumn id="21" name="MSA - Head of Department"/>
+    <tableColumn id="1" name="A" dataDxfId="64"/>
+    <tableColumn id="2" name="Primary Group" dataDxfId="63"/>
+    <tableColumn id="5" name="Salut." dataDxfId="62"/>
+    <tableColumn id="6" name="Last Name" dataDxfId="61"/>
+    <tableColumn id="7" name="First Name" dataDxfId="60"/>
+    <tableColumn id="45" name="Middle Name" dataDxfId="59"/>
+    <tableColumn id="22" name="Degree" dataDxfId="58"/>
+    <tableColumn id="54" name="Employee Type" dataDxfId="57"/>
+    <tableColumn id="28" name="Administrative Title" dataDxfId="56"/>
+    <tableColumn id="44" name="Administrative - Institution" dataDxfId="55"/>
+    <tableColumn id="31" name="Administrative - Department" dataDxfId="54"/>
+    <tableColumn id="24" name="Administrative - Division" dataDxfId="53"/>
+    <tableColumn id="25" name="Administrative - Service" dataDxfId="52"/>
+    <tableColumn id="33" name="Administrative - Head of this Department" dataDxfId="51"/>
+    <tableColumn id="35" name="Administrative - Head of this Division" dataDxfId="50"/>
+    <tableColumn id="34" name="Administrative - Head of this Service" dataDxfId="49"/>
+    <tableColumn id="20" name="Medical Staff Appointment (MSA) Title" dataDxfId="48"/>
+    <tableColumn id="62" name="MSA - Institution" dataDxfId="47"/>
+    <tableColumn id="61" name="MSA - Department" dataDxfId="46"/>
+    <tableColumn id="43" name="MSA - Division" dataDxfId="45"/>
+    <tableColumn id="42" name="MSA - Service" dataDxfId="44"/>
+    <tableColumn id="21" name="MSA - Head of Department" dataDxfId="43"/>
     <tableColumn id="18" name="MSA - Head of Division" dataDxfId="42"/>
     <tableColumn id="19" name="MSA - Head of Service" dataDxfId="41"/>
     <tableColumn id="29" name="Academic Title" dataDxfId="40"/>
@@ -2209,31 +2431,31 @@
     <tableColumn id="11" name="Office Location" dataDxfId="27"/>
     <tableColumn id="12" name="E-mail Address" dataDxfId="26" dataCellStyle="Hyperlink"/>
     <tableColumn id="30" name="CWID" dataDxfId="25"/>
-    <tableColumn id="3" name="Certifying Board Organization" dataDxfId="0"/>
-    <tableColumn id="36" name="Board Certification - Specialty" dataDxfId="24"/>
-    <tableColumn id="37" name="Board Certification - Date Issued" dataDxfId="23"/>
-    <tableColumn id="46" name="Board Certification - Expiration Date" dataDxfId="22"/>
-    <tableColumn id="47" name="Board Certification - Recertification Date" dataDxfId="21"/>
-    <tableColumn id="32" name="NYPH Code" dataDxfId="20"/>
-    <tableColumn id="39" name="License state" dataDxfId="19"/>
-    <tableColumn id="40" name="License number" dataDxfId="18"/>
-    <tableColumn id="41" name="License expiration" dataDxfId="17"/>
-    <tableColumn id="17" name="Assistants" dataDxfId="16"/>
-    <tableColumn id="48" name="Administrative Comment - Category" dataDxfId="15"/>
-    <tableColumn id="49" name="Administrative Comment - Name" dataDxfId="14"/>
-    <tableColumn id="50" name="Administrative Comment - Comment" dataDxfId="13"/>
-    <tableColumn id="51" name="Identifier - Type" dataDxfId="12"/>
-    <tableColumn id="52" name="Identifier" dataDxfId="11"/>
-    <tableColumn id="53" name="Identifier - link" dataDxfId="10"/>
-    <tableColumn id="55" name="Certificate of Qualification - Code" dataDxfId="9"/>
-    <tableColumn id="56" name="Certificate of Qualification - Serial Number" dataDxfId="8"/>
-    <tableColumn id="57" name="Certificate of Qualification - Expiration Date" dataDxfId="7"/>
-    <tableColumn id="59" name="CLIA - Number" dataDxfId="6"/>
-    <tableColumn id="58" name="CLIA - Expiration Date" dataDxfId="5"/>
-    <tableColumn id="60" name="PFI" dataDxfId="4"/>
-    <tableColumn id="68" name="POPS Link" dataDxfId="3"/>
-    <tableColumn id="70" name="Pubmed Link" dataDxfId="2"/>
-    <tableColumn id="69" name="VIVO link" dataDxfId="1"/>
+    <tableColumn id="3" name="Certifying Board Organization" dataDxfId="24"/>
+    <tableColumn id="36" name="Board Certification - Specialty" dataDxfId="23"/>
+    <tableColumn id="37" name="Board Certification - Date Issued" dataDxfId="22"/>
+    <tableColumn id="46" name="Board Certification - Expiration Date" dataDxfId="21"/>
+    <tableColumn id="47" name="Board Certification - Recertification Date" dataDxfId="20"/>
+    <tableColumn id="32" name="NYPH Code" dataDxfId="19"/>
+    <tableColumn id="39" name="License state" dataDxfId="18"/>
+    <tableColumn id="40" name="License number" dataDxfId="17"/>
+    <tableColumn id="41" name="License expiration" dataDxfId="16"/>
+    <tableColumn id="17" name="Assistants" dataDxfId="15"/>
+    <tableColumn id="48" name="Administrative Comment - Category" dataDxfId="14"/>
+    <tableColumn id="49" name="Administrative Comment - Name" dataDxfId="13"/>
+    <tableColumn id="50" name="Administrative Comment - Comment" dataDxfId="5"/>
+    <tableColumn id="51" name="Identifier - Type" dataDxfId="4"/>
+    <tableColumn id="52" name="Identifier" dataDxfId="3"/>
+    <tableColumn id="53" name="Identifier - link" dataDxfId="12"/>
+    <tableColumn id="55" name="Certificate of Qualification - Code" dataDxfId="11"/>
+    <tableColumn id="56" name="Certificate of Qualification - Serial Number" dataDxfId="10"/>
+    <tableColumn id="57" name="Certificate of Qualification - Expiration Date" dataDxfId="9"/>
+    <tableColumn id="59" name="CLIA - Number" dataDxfId="8"/>
+    <tableColumn id="58" name="CLIA - Expiration Date" dataDxfId="7"/>
+    <tableColumn id="60" name="PFI" dataDxfId="6"/>
+    <tableColumn id="68" name="POPS Link" dataDxfId="2"/>
+    <tableColumn id="70" name="Pubmed Link" dataDxfId="1"/>
+    <tableColumn id="69" name="VIVO link" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2494,7 +2716,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2502,12 +2724,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BV2"/>
+  <dimension ref="A1:BV3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="AE1" activePane="topRight" state="frozen"/>
+      <pane xSplit="3" topLeftCell="AF1" activePane="topRight" state="frozen"/>
       <selection activeCell="C89" sqref="C89"/>
-      <selection pane="topRight" activeCell="AN2" sqref="AN2"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2520,7 +2742,7 @@
     <col min="6" max="6" width="10.85546875" style="7" customWidth="1"/>
     <col min="7" max="7" width="11.140625" style="7" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="48" style="15" customWidth="1"/>
+    <col min="9" max="9" width="48" style="14" customWidth="1"/>
     <col min="10" max="10" width="31.85546875" style="7" customWidth="1"/>
     <col min="11" max="11" width="19.28515625" style="7" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" style="7" customWidth="1"/>
@@ -2528,14 +2750,14 @@
     <col min="14" max="14" width="43.140625" style="7" customWidth="1"/>
     <col min="15" max="15" width="24.42578125" style="7" customWidth="1"/>
     <col min="16" max="16" width="42.42578125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="28.7109375" style="16" customWidth="1"/>
+    <col min="17" max="17" width="28.7109375" style="15" customWidth="1"/>
     <col min="18" max="19" width="13.85546875" customWidth="1"/>
     <col min="20" max="20" width="16.140625" customWidth="1"/>
     <col min="21" max="21" width="20" customWidth="1"/>
     <col min="22" max="22" width="17.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17.7109375" style="7" customWidth="1"/>
-    <col min="25" max="25" width="44.85546875" style="15" customWidth="1"/>
+    <col min="25" max="25" width="44.85546875" style="14" customWidth="1"/>
     <col min="26" max="26" width="44.85546875" style="7" customWidth="1"/>
     <col min="27" max="27" width="13.7109375" style="7" customWidth="1"/>
     <col min="28" max="31" width="37.42578125" style="7" customWidth="1"/>
@@ -2596,88 +2818,88 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y1" s="13" t="s">
-        <v>22</v>
+        <v>53</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>5</v>
@@ -2689,7 +2911,7 @@
         <v>6</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="AL1" s="1" t="s">
         <v>8</v>
@@ -2698,261 +2920,322 @@
         <v>4</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="AQ1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AR1" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="AS1" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="AU1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AX1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="BB1" s="1" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="BE1" s="11" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="BF1" s="11" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="BG1" s="11" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="BH1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="BI1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="BK1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="BI1" s="9" t="s">
+      <c r="BL1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="BM1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="BJ1" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="BK1" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="BL1" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="BM1" s="9" t="s">
-        <v>100</v>
-      </c>
     </row>
-    <row r="2" spans="1:65" s="1" customFormat="1" ht="135">
+    <row r="2" spans="1:65" s="1" customFormat="1" ht="75">
       <c r="A2" s="5" t="b">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>92</v>
+        <v>72</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>97</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="S2" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="U2" s="17" t="s">
-        <v>97</v>
-      </c>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y2" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>94</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z2" s="3"/>
       <c r="AA2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB2" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC2" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD2" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE2" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>39</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
       <c r="AH2" s="3" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
       <c r="AL2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="AM2" s="8" t="s">
-        <v>14</v>
+        <v>80</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>70</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="AO2" s="3"/>
+      <c r="AP2" s="3"/>
+      <c r="AQ2" s="3"/>
+      <c r="AR2" s="3"/>
       <c r="AS2" s="3"/>
-      <c r="AT2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="AT2" s="3"/>
+      <c r="AU2" s="3"/>
+      <c r="AV2" s="3"/>
+      <c r="AW2" s="3"/>
       <c r="AX2" s="3"/>
-      <c r="AY2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA2" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="AY2" s="3"/>
+      <c r="AZ2" s="3"/>
+      <c r="BA2" s="3"/>
       <c r="BB2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>69</v>
+        <v>82</v>
+      </c>
+      <c r="BC2" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="BD2" s="3"/>
-      <c r="BE2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="BF2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BG2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="BH2" s="3"/>
+      <c r="BE2" s="3"/>
+      <c r="BF2" s="3"/>
+      <c r="BG2" s="3"/>
+      <c r="BH2" s="10"/>
       <c r="BI2" s="10"/>
       <c r="BJ2" s="10"/>
-      <c r="BK2" s="10"/>
-      <c r="BL2" s="8" t="s">
-        <v>103</v>
+      <c r="BK2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="BL2" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="BM2" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:65" s="1" customFormat="1" ht="45">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>102</v>
       </c>
+      <c r="E3" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="19"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="R3" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z3" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC3" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD3" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
+      <c r="AH3" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI3" s="19"/>
+      <c r="AJ3" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="AK3" s="19"/>
+      <c r="AL3" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM3" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="AN3" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO3" s="19"/>
+      <c r="AP3" s="19"/>
+      <c r="AQ3" s="19"/>
+      <c r="AR3" s="19"/>
+      <c r="AS3" s="19"/>
+      <c r="AT3" s="19"/>
+      <c r="AU3" s="19"/>
+      <c r="AV3" s="19"/>
+      <c r="AX3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AY3" s="19"/>
+      <c r="AZ3" s="19"/>
+      <c r="BA3" s="19"/>
+      <c r="BB3" s="19"/>
+      <c r="BC3" s="19"/>
+      <c r="BD3" s="19"/>
+      <c r="BE3" s="19"/>
+      <c r="BF3" s="19"/>
+      <c r="BG3" s="19"/>
+      <c r="BH3" s="10"/>
+      <c r="BI3" s="10"/>
+      <c r="BJ3" s="10"/>
+      <c r="BK3" s="10"/>
+      <c r="BL3" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BL2" r:id="rId1"/>
-    <hyperlink ref="AM2" r:id="rId2"/>
+    <hyperlink ref="AM3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
working on user gen
</commit_message>
<xml_diff>
--- a/Scanorders2/src/Oleg/UserdirectoryBundle/Util/UsersFullTest.xlsx
+++ b/Scanorders2/src/Oleg/UserdirectoryBundle/Util/UsersFullTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="51195" windowHeight="24180"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="51195" windowHeight="24120"/>
   </bookViews>
   <sheets>
     <sheet name="owssvr.dll" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="129">
   <si>
     <t>A</t>
   </si>
@@ -237,66 +237,12 @@
     <t>Pubmed Link</t>
   </si>
   <si>
-    <t>Certifying Board Organization</t>
-  </si>
-  <si>
-    <t>Anatomic Pathology Faculty</t>
-  </si>
-  <si>
-    <t>Victor</t>
-  </si>
-  <si>
     <t>MD</t>
   </si>
   <si>
-    <t>Medical Director of Informatics</t>
-  </si>
-  <si>
-    <t>New York-Presbyterian Hospital</t>
-  </si>
-  <si>
     <t>Pathology and Laboratory Medicine</t>
   </si>
   <si>
-    <t>Pathology Informatics</t>
-  </si>
-  <si>
-    <t>Assistant Professor of Pathology and Laboratory Medicine; Assistant Professor of Public Health</t>
-  </si>
-  <si>
-    <t>3/1/2010</t>
-  </si>
-  <si>
-    <t>(646) 962-2997; (646) 592-3803; (212) 746-5820</t>
-  </si>
-  <si>
-    <t>(212) 746-2113</t>
-  </si>
-  <si>
-    <t>K-505</t>
-  </si>
-  <si>
-    <t>vib9020@med.cornell.edu</t>
-  </si>
-  <si>
-    <t>EIN</t>
-  </si>
-  <si>
-    <t>200-31-063</t>
-  </si>
-  <si>
-    <t>http://weillcornell.org/vbrodsky</t>
-  </si>
-  <si>
-    <t>http://www.ncbi.nlm.nih.gov/pubmed?term=Brodsky%20V%5BAuthor%5D&amp;cauthor=true&amp;cauthor_uid=23024889</t>
-  </si>
-  <si>
-    <t>http://vivo.med.cornell.edu/display/cwid-vib9020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. </t>
-  </si>
-  <si>
     <t>Alain</t>
   </si>
   <si>
@@ -330,23 +276,155 @@
     <t>Gaud, Melody</t>
   </si>
   <si>
-    <t>vib9020Test3</t>
-  </si>
-  <si>
-    <t>Brodsky3</t>
-  </si>
-  <si>
-    <t>alb9003Test4</t>
-  </si>
-  <si>
-    <t>Borczuk4</t>
+    <t>Donna</t>
+  </si>
+  <si>
+    <t>Senior Administrative Coordinator; Residency/Fellowship Coordinator</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>(212) 746-7365</t>
+  </si>
+  <si>
+    <t>(212) 746-8192</t>
+  </si>
+  <si>
+    <t>C-302</t>
+  </si>
+  <si>
+    <t>dmgalvin@med.cornell.edu</t>
+  </si>
+  <si>
+    <t>alb9003Test1</t>
+  </si>
+  <si>
+    <t>Borczuk1</t>
+  </si>
+  <si>
+    <t>Galvin1</t>
+  </si>
+  <si>
+    <t>dmgalvinTest1</t>
+  </si>
+  <si>
+    <t>Ethel</t>
+  </si>
+  <si>
+    <t>MD; PhD</t>
+  </si>
+  <si>
+    <t>Assistant Director, Molecular Hematopathology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New York-Presbyterian Hospital; New York-Presbyterian Hospital; </t>
+  </si>
+  <si>
+    <t>Pathology and Laboratory Medicine; Pathology and Laboratory Medicine</t>
+  </si>
+  <si>
+    <t>Hematopathology; Molecular and Genomic Pathology</t>
+  </si>
+  <si>
+    <t>Molecular Hematopathology; Molecular Hematopathology</t>
+  </si>
+  <si>
+    <t>Yes; Yes</t>
+  </si>
+  <si>
+    <t>Attending Pathologist</t>
+  </si>
+  <si>
+    <t>Professor of Pathology and Laboratory Medicine</t>
+  </si>
+  <si>
+    <t>3/1/1994</t>
+  </si>
+  <si>
+    <t>Weill Cornell Medical College; Weill Cornell Medical College; Weill Cornell Medical College</t>
+  </si>
+  <si>
+    <t>Viral Oncogenesis</t>
+  </si>
+  <si>
+    <t>(212) 746-8838</t>
+  </si>
+  <si>
+    <t>(212) 746-4483</t>
+  </si>
+  <si>
+    <t>C-410B</t>
+  </si>
+  <si>
+    <t>ecesarm@med.cornell.edu</t>
+  </si>
+  <si>
+    <t>Anatomic Pathology; Molecular Genetic Pathology</t>
+  </si>
+  <si>
+    <t>11/20/1991; 9/24/2007</t>
+  </si>
+  <si>
+    <t>null; 12/31/2017</t>
+  </si>
+  <si>
+    <t>CE018</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>187177-1</t>
+  </si>
+  <si>
+    <t>9/30/2015</t>
+  </si>
+  <si>
+    <t>Faculty Database - Donna</t>
+  </si>
+  <si>
+    <t>Special Appointment Notes</t>
+  </si>
+  <si>
+    <t>2007 Professor</t>
+  </si>
+  <si>
+    <t>NPI;EIN</t>
+  </si>
+  <si>
+    <t>1770523987; 200-08-083</t>
+  </si>
+  <si>
+    <t>CESAE1</t>
+  </si>
+  <si>
+    <t>CQP90583</t>
+  </si>
+  <si>
+    <t>2/8/2016</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/pubmed?term=Cesarman%20E%5BAuthor%5D&amp;cauthor=true&amp;cauthor_uid=22507788</t>
+  </si>
+  <si>
+    <t>http://vivo.med.cornell.edu/display/cwid-ecesarm</t>
+  </si>
+  <si>
+    <t>Hematopathology Faculty</t>
+  </si>
+  <si>
+    <t>ecesarm2</t>
+  </si>
+  <si>
+    <t>Cesarman2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,8 +596,27 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -711,8 +808,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FFDDEBF7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -838,6 +941,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF9BC2E6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9BC2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="288">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1129,7 +1269,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1199,6 +1339,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1492,7 +1659,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="65">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1545,36 +1712,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -1681,6 +1818,36 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1904,16 +2071,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2385,53 +2542,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr.dll" displayName="Table_owssvr.dll" ref="A1:BM2" totalsRowShown="0" headerRowDxfId="65">
-  <autoFilter ref="A1:BM2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr.dll" displayName="Table_owssvr.dll" ref="A1:BL2" insertRow="1" totalsRowShown="0" headerRowDxfId="64">
+  <autoFilter ref="A1:BL2"/>
   <sortState ref="A2:BL356">
     <sortCondition ref="D1:D356"/>
   </sortState>
-  <tableColumns count="65">
-    <tableColumn id="1" name="A" dataDxfId="64"/>
-    <tableColumn id="2" name="Primary Group" dataDxfId="63"/>
-    <tableColumn id="5" name="Salut." dataDxfId="62"/>
-    <tableColumn id="6" name="Last Name" dataDxfId="61"/>
-    <tableColumn id="7" name="First Name" dataDxfId="60"/>
-    <tableColumn id="45" name="Middle Name" dataDxfId="59"/>
-    <tableColumn id="22" name="Degree" dataDxfId="58"/>
-    <tableColumn id="54" name="Employee Type" dataDxfId="57"/>
-    <tableColumn id="28" name="Administrative Title" dataDxfId="56"/>
-    <tableColumn id="44" name="Administrative - Institution" dataDxfId="55"/>
-    <tableColumn id="31" name="Administrative - Department" dataDxfId="54"/>
-    <tableColumn id="24" name="Administrative - Division" dataDxfId="53"/>
-    <tableColumn id="25" name="Administrative - Service" dataDxfId="52"/>
-    <tableColumn id="33" name="Administrative - Head of this Department" dataDxfId="51"/>
-    <tableColumn id="35" name="Administrative - Head of this Division" dataDxfId="50"/>
-    <tableColumn id="34" name="Administrative - Head of this Service" dataDxfId="49"/>
-    <tableColumn id="20" name="Medical Staff Appointment (MSA) Title" dataDxfId="48"/>
-    <tableColumn id="62" name="MSA - Institution" dataDxfId="47"/>
-    <tableColumn id="61" name="MSA - Department" dataDxfId="46"/>
-    <tableColumn id="43" name="MSA - Division" dataDxfId="45"/>
-    <tableColumn id="42" name="MSA - Service" dataDxfId="44"/>
-    <tableColumn id="21" name="MSA - Head of Department" dataDxfId="43"/>
-    <tableColumn id="18" name="MSA - Head of Division" dataDxfId="42"/>
-    <tableColumn id="19" name="MSA - Head of Service" dataDxfId="41"/>
-    <tableColumn id="29" name="Academic Title" dataDxfId="40"/>
-    <tableColumn id="63" name="Academic Appointment - Faculty Track" dataDxfId="39"/>
-    <tableColumn id="38" name="Academic Appointment start date" dataDxfId="38"/>
-    <tableColumn id="67" name="Academic Appt - Institution" dataDxfId="37"/>
-    <tableColumn id="66" name="Academic Appt - Department" dataDxfId="36"/>
-    <tableColumn id="65" name="Academic Appt - Division" dataDxfId="35"/>
-    <tableColumn id="64" name="Academic Appt - Service" dataDxfId="34"/>
-    <tableColumn id="26" name="Research Lab Title" dataDxfId="33"/>
-    <tableColumn id="27" name="Principle Investigator of this Lab" dataDxfId="32"/>
-    <tableColumn id="9" name="Business Phone" dataDxfId="31"/>
-    <tableColumn id="13" name="Fax Number" dataDxfId="30"/>
-    <tableColumn id="10" name="Pager" dataDxfId="29"/>
-    <tableColumn id="23" name="Intercom" dataDxfId="28"/>
-    <tableColumn id="11" name="Office Location" dataDxfId="27"/>
-    <tableColumn id="12" name="E-mail Address" dataDxfId="26" dataCellStyle="Hyperlink"/>
-    <tableColumn id="30" name="CWID" dataDxfId="25"/>
-    <tableColumn id="3" name="Certifying Board Organization" dataDxfId="24"/>
+  <tableColumns count="64">
+    <tableColumn id="1" name="A" dataDxfId="63"/>
+    <tableColumn id="2" name="Primary Group" dataDxfId="62"/>
+    <tableColumn id="5" name="Salut." dataDxfId="61"/>
+    <tableColumn id="6" name="Last Name" dataDxfId="60"/>
+    <tableColumn id="7" name="First Name" dataDxfId="59"/>
+    <tableColumn id="45" name="Middle Name" dataDxfId="58"/>
+    <tableColumn id="22" name="Degree" dataDxfId="57"/>
+    <tableColumn id="54" name="Employee Type" dataDxfId="56"/>
+    <tableColumn id="28" name="Administrative Title" dataDxfId="55"/>
+    <tableColumn id="44" name="Administrative - Institution" dataDxfId="54"/>
+    <tableColumn id="31" name="Administrative - Department" dataDxfId="53"/>
+    <tableColumn id="24" name="Administrative - Division" dataDxfId="52"/>
+    <tableColumn id="25" name="Administrative - Service" dataDxfId="51"/>
+    <tableColumn id="33" name="Administrative - Head of this Department" dataDxfId="50"/>
+    <tableColumn id="35" name="Administrative - Head of this Division" dataDxfId="49"/>
+    <tableColumn id="34" name="Administrative - Head of this Service" dataDxfId="48"/>
+    <tableColumn id="20" name="Medical Staff Appointment (MSA) Title" dataDxfId="47"/>
+    <tableColumn id="62" name="MSA - Institution" dataDxfId="46"/>
+    <tableColumn id="61" name="MSA - Department" dataDxfId="45"/>
+    <tableColumn id="43" name="MSA - Division" dataDxfId="44"/>
+    <tableColumn id="42" name="MSA - Service" dataDxfId="43"/>
+    <tableColumn id="21" name="MSA - Head of Department" dataDxfId="42"/>
+    <tableColumn id="18" name="MSA - Head of Division" dataDxfId="41"/>
+    <tableColumn id="19" name="MSA - Head of Service" dataDxfId="40"/>
+    <tableColumn id="29" name="Academic Title" dataDxfId="39"/>
+    <tableColumn id="63" name="Academic Appointment - Faculty Track" dataDxfId="38"/>
+    <tableColumn id="38" name="Academic Appointment start date" dataDxfId="37"/>
+    <tableColumn id="67" name="Academic Appt - Institution" dataDxfId="36"/>
+    <tableColumn id="66" name="Academic Appt - Department" dataDxfId="35"/>
+    <tableColumn id="65" name="Academic Appt - Division" dataDxfId="34"/>
+    <tableColumn id="64" name="Academic Appt - Service" dataDxfId="33"/>
+    <tableColumn id="26" name="Research Lab Title" dataDxfId="32"/>
+    <tableColumn id="27" name="Principle Investigator of this Lab" dataDxfId="31"/>
+    <tableColumn id="9" name="Business Phone" dataDxfId="30"/>
+    <tableColumn id="13" name="Fax Number" dataDxfId="29"/>
+    <tableColumn id="10" name="Pager" dataDxfId="28"/>
+    <tableColumn id="23" name="Intercom" dataDxfId="27"/>
+    <tableColumn id="11" name="Office Location" dataDxfId="26"/>
+    <tableColumn id="12" name="E-mail Address" dataDxfId="25" dataCellStyle="Hyperlink"/>
+    <tableColumn id="30" name="CWID" dataDxfId="24"/>
     <tableColumn id="36" name="Board Certification - Specialty" dataDxfId="23"/>
     <tableColumn id="37" name="Board Certification - Date Issued" dataDxfId="22"/>
     <tableColumn id="46" name="Board Certification - Expiration Date" dataDxfId="21"/>
@@ -2443,16 +2599,16 @@
     <tableColumn id="17" name="Assistants" dataDxfId="15"/>
     <tableColumn id="48" name="Administrative Comment - Category" dataDxfId="14"/>
     <tableColumn id="49" name="Administrative Comment - Name" dataDxfId="13"/>
-    <tableColumn id="50" name="Administrative Comment - Comment" dataDxfId="5"/>
-    <tableColumn id="51" name="Identifier - Type" dataDxfId="4"/>
-    <tableColumn id="52" name="Identifier" dataDxfId="3"/>
-    <tableColumn id="53" name="Identifier - link" dataDxfId="12"/>
-    <tableColumn id="55" name="Certificate of Qualification - Code" dataDxfId="11"/>
-    <tableColumn id="56" name="Certificate of Qualification - Serial Number" dataDxfId="10"/>
-    <tableColumn id="57" name="Certificate of Qualification - Expiration Date" dataDxfId="9"/>
-    <tableColumn id="59" name="CLIA - Number" dataDxfId="8"/>
-    <tableColumn id="58" name="CLIA - Expiration Date" dataDxfId="7"/>
-    <tableColumn id="60" name="PFI" dataDxfId="6"/>
+    <tableColumn id="50" name="Administrative Comment - Comment" dataDxfId="12"/>
+    <tableColumn id="51" name="Identifier - Type" dataDxfId="11"/>
+    <tableColumn id="52" name="Identifier" dataDxfId="10"/>
+    <tableColumn id="53" name="Identifier - link" dataDxfId="9"/>
+    <tableColumn id="55" name="Certificate of Qualification - Code" dataDxfId="8"/>
+    <tableColumn id="56" name="Certificate of Qualification - Serial Number" dataDxfId="7"/>
+    <tableColumn id="57" name="Certificate of Qualification - Expiration Date" dataDxfId="6"/>
+    <tableColumn id="59" name="CLIA - Number" dataDxfId="5"/>
+    <tableColumn id="58" name="CLIA - Expiration Date" dataDxfId="4"/>
+    <tableColumn id="60" name="PFI" dataDxfId="3"/>
     <tableColumn id="68" name="POPS Link" dataDxfId="2"/>
     <tableColumn id="70" name="Pubmed Link" dataDxfId="1"/>
     <tableColumn id="69" name="VIVO link" dataDxfId="0"/>
@@ -2724,12 +2880,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BV3"/>
+  <dimension ref="A1:BU5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="AF1" activePane="topRight" state="frozen"/>
+      <pane xSplit="3" topLeftCell="AG1" activePane="topRight" state="frozen"/>
       <selection activeCell="C89" sqref="C89"/>
-      <selection pane="topRight" activeCell="D3" sqref="D3"/>
+      <selection pane="topRight" activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2769,39 +2925,39 @@
     <col min="37" max="37" width="30.28515625" style="7" customWidth="1"/>
     <col min="38" max="38" width="14" style="7" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="16" style="7" customWidth="1"/>
-    <col min="40" max="41" width="17.28515625" style="7" customWidth="1"/>
-    <col min="44" max="44" width="21.85546875" style="7" customWidth="1"/>
-    <col min="45" max="45" width="30.140625" style="7" customWidth="1"/>
-    <col min="46" max="46" width="21.85546875" style="7" customWidth="1"/>
-    <col min="47" max="47" width="26.7109375" style="7" customWidth="1"/>
-    <col min="51" max="51" width="14.140625" customWidth="1"/>
-    <col min="54" max="54" width="20.28515625" customWidth="1"/>
-    <col min="55" max="55" width="34.140625" style="7" customWidth="1"/>
-    <col min="56" max="56" width="11.85546875" style="7" customWidth="1"/>
-    <col min="57" max="58" width="8.85546875" style="7"/>
-    <col min="59" max="59" width="15.28515625" style="7" customWidth="1"/>
-    <col min="60" max="60" width="25" style="7" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="24.140625" style="7" customWidth="1"/>
-    <col min="62" max="62" width="23.140625" style="7" customWidth="1"/>
-    <col min="63" max="63" width="31.140625" style="7" customWidth="1"/>
-    <col min="64" max="64" width="23.140625" style="7" customWidth="1"/>
-    <col min="65" max="65" width="18.7109375" customWidth="1"/>
-    <col min="66" max="67" width="21.85546875" style="7" customWidth="1"/>
-    <col min="68" max="68" width="26" style="7" customWidth="1"/>
-    <col min="69" max="70" width="16.28515625" style="7" customWidth="1"/>
-    <col min="71" max="71" width="18.28515625" style="9" customWidth="1"/>
-    <col min="72" max="72" width="23.85546875" style="9" customWidth="1"/>
-    <col min="73" max="73" width="34.140625" style="9" customWidth="1"/>
-    <col min="74" max="74" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="39.28515625" style="6" customWidth="1"/>
-    <col min="76" max="76" width="8.85546875" style="6"/>
-    <col min="77" max="77" width="23" style="6" customWidth="1"/>
-    <col min="78" max="81" width="8.85546875" style="6"/>
-    <col min="82" max="82" width="21.42578125" style="6" customWidth="1"/>
-    <col min="83" max="16384" width="8.85546875" style="6"/>
+    <col min="40" max="40" width="17.28515625" style="7" customWidth="1"/>
+    <col min="43" max="43" width="21.85546875" style="7" customWidth="1"/>
+    <col min="44" max="44" width="30.140625" style="7" customWidth="1"/>
+    <col min="45" max="45" width="21.85546875" style="7" customWidth="1"/>
+    <col min="46" max="46" width="26.7109375" style="7" customWidth="1"/>
+    <col min="50" max="50" width="14.140625" customWidth="1"/>
+    <col min="53" max="53" width="20.28515625" customWidth="1"/>
+    <col min="54" max="54" width="34.140625" style="7" customWidth="1"/>
+    <col min="55" max="55" width="11.85546875" style="7" customWidth="1"/>
+    <col min="56" max="57" width="8.85546875" style="7"/>
+    <col min="58" max="58" width="15.28515625" style="7" customWidth="1"/>
+    <col min="59" max="59" width="25" style="7" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="24.140625" style="7" customWidth="1"/>
+    <col min="61" max="61" width="23.140625" style="7" customWidth="1"/>
+    <col min="62" max="62" width="31.140625" style="7" customWidth="1"/>
+    <col min="63" max="63" width="23.140625" style="7" customWidth="1"/>
+    <col min="64" max="64" width="18.7109375" customWidth="1"/>
+    <col min="65" max="66" width="21.85546875" style="7" customWidth="1"/>
+    <col min="67" max="67" width="26" style="7" customWidth="1"/>
+    <col min="68" max="69" width="16.28515625" style="7" customWidth="1"/>
+    <col min="70" max="70" width="18.28515625" style="9" customWidth="1"/>
+    <col min="71" max="71" width="23.85546875" style="9" customWidth="1"/>
+    <col min="72" max="72" width="34.140625" style="9" customWidth="1"/>
+    <col min="73" max="73" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="39.28515625" style="6" customWidth="1"/>
+    <col min="75" max="75" width="8.85546875" style="6"/>
+    <col min="76" max="76" width="23" style="6" customWidth="1"/>
+    <col min="77" max="80" width="8.85546875" style="6"/>
+    <col min="81" max="81" width="21.42578125" style="6" customWidth="1"/>
+    <col min="82" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" s="1" customFormat="1" ht="90">
+    <row r="1" spans="1:64" s="1" customFormat="1" ht="90">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2923,116 +3079,91 @@
         <v>16</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="BD1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="BD1" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="BE1" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="BF1" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="BG1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="BH1" s="11" t="s">
         <v>41</v>
       </c>
+      <c r="BH1" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="BI1" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="BJ1" s="9" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="BK1" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BL1" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="BM1" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:65" s="1" customFormat="1" ht="75">
-      <c r="A2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>70</v>
-      </c>
+    <row r="2" spans="1:64" s="1" customFormat="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>75</v>
-      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -3044,39 +3175,23 @@
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
-      <c r="X2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y2" s="13" t="s">
-        <v>76</v>
-      </c>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="13"/>
       <c r="Z2" s="3"/>
-      <c r="AA2" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="AA2" s="3"/>
       <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
       <c r="AG2" s="3"/>
-      <c r="AH2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
-      <c r="AL2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="3"/>
       <c r="AO2" s="3"/>
       <c r="AP2" s="3"/>
       <c r="AQ2" s="3"/>
@@ -3090,57 +3205,44 @@
       <c r="AY2" s="3"/>
       <c r="AZ2" s="3"/>
       <c r="BA2" s="3"/>
-      <c r="BB2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="BC2" s="17" t="s">
-        <v>83</v>
-      </c>
+      <c r="BB2" s="17"/>
+      <c r="BC2" s="3"/>
       <c r="BD2" s="3"/>
       <c r="BE2" s="3"/>
       <c r="BF2" s="3"/>
-      <c r="BG2" s="3"/>
+      <c r="BG2" s="10"/>
       <c r="BH2" s="10"/>
       <c r="BI2" s="10"/>
       <c r="BJ2" s="10"/>
-      <c r="BK2" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="BL2" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="BM2" s="10" t="s">
-        <v>86</v>
-      </c>
+      <c r="BK2" s="10"/>
+      <c r="BL2" s="10"/>
     </row>
-    <row r="3" spans="1:65" s="1" customFormat="1" ht="45">
+    <row r="3" spans="1:64" s="1" customFormat="1" ht="45">
       <c r="A3" s="5"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="18" t="s">
-        <v>87</v>
-      </c>
+      <c r="C3" s="18"/>
       <c r="D3" s="19" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="20" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="M3" s="19"/>
       <c r="N3" s="22"/>
@@ -3149,16 +3251,16 @@
       </c>
       <c r="P3" s="22"/>
       <c r="Q3" s="23" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="R3" s="24" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="T3" s="19" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="U3" s="19"/>
       <c r="V3" s="19"/>
@@ -3167,40 +3269,40 @@
         <v>24</v>
       </c>
       <c r="Y3" s="23" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="Z3" s="19" t="s">
         <v>64</v>
       </c>
       <c r="AA3" s="19"/>
       <c r="AB3" s="24" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="AC3" s="24" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="AD3" s="24" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="AE3" s="24"/>
       <c r="AF3" s="19"/>
       <c r="AG3" s="19"/>
       <c r="AH3" s="19" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="AI3" s="19"/>
       <c r="AJ3" s="19" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="AK3" s="19"/>
       <c r="AL3" s="19" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="AM3" s="8" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="AN3" s="19" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="AO3" s="19"/>
       <c r="AP3" s="19"/>
@@ -3209,10 +3311,10 @@
       <c r="AS3" s="19"/>
       <c r="AT3" s="19"/>
       <c r="AU3" s="19"/>
-      <c r="AV3" s="19"/>
-      <c r="AX3" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="AW3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX3" s="19"/>
       <c r="AY3" s="19"/>
       <c r="AZ3" s="19"/>
       <c r="BA3" s="19"/>
@@ -3221,12 +3323,261 @@
       <c r="BD3" s="19"/>
       <c r="BE3" s="19"/>
       <c r="BF3" s="19"/>
-      <c r="BG3" s="19"/>
+      <c r="BG3" s="10"/>
       <c r="BH3" s="10"/>
       <c r="BI3" s="10"/>
       <c r="BJ3" s="10"/>
       <c r="BK3" s="10"/>
-      <c r="BL3" s="10"/>
+    </row>
+    <row r="4" spans="1:64" ht="45">
+      <c r="C4" s="25"/>
+      <c r="D4" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M4" s="16"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI4" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ4" s="16"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM4" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN4" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO4" s="16"/>
+      <c r="AP4" s="16"/>
+      <c r="AQ4" s="16"/>
+      <c r="AR4" s="16"/>
+      <c r="AS4" s="16"/>
+      <c r="AT4" s="16"/>
+      <c r="AU4" s="16"/>
+      <c r="AV4" s="16"/>
+      <c r="AW4" s="16"/>
+      <c r="AX4" s="16"/>
+      <c r="AY4" s="16"/>
+      <c r="AZ4" s="16"/>
+      <c r="BA4" s="16"/>
+      <c r="BB4" s="16"/>
+      <c r="BC4" s="16"/>
+      <c r="BD4" s="16"/>
+      <c r="BE4" s="16"/>
+      <c r="BF4" s="16"/>
+      <c r="BG4" s="30"/>
+      <c r="BH4" s="30"/>
+      <c r="BI4" s="30"/>
+      <c r="BJ4" s="30"/>
+      <c r="BK4" s="31"/>
+    </row>
+    <row r="5" spans="1:64" s="1" customFormat="1" ht="135">
+      <c r="A5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="R5" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="S5" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="T5" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="U5" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y5" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB5" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC5" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD5" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE5" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM5" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN5" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO5" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP5" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AQ5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AR5" s="3"/>
+      <c r="AS5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AV5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AW5" s="3"/>
+      <c r="AX5" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AY5" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AZ5" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="BA5" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC5" s="3"/>
+      <c r="BD5" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="BE5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="BF5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="BG5" s="3"/>
+      <c r="BH5" s="10"/>
+      <c r="BI5" s="10"/>
+      <c r="BJ5" s="10"/>
+      <c r="BK5" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="BL5" s="10" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>